<commit_message>
Changed the sprint2 sprint breakdown records to include the dependence of the tasks (was missing from the chart). Fixed the planned burndown chart in the sprint3 actual execution (was graphing the actual instead of planned)
</commit_message>
<xml_diff>
--- a/Sprint Backlog/Sprint2/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
+++ b/Sprint Backlog/Sprint2/Planning and Burndown/Actual Execution and Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Sprint Backlog\Sprint2\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F82F15-5E44-475A-A032-42EE848BEDE6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74856157-83F0-44FF-B1A6-128F8B96B5EC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>User Stories</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>7</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Column1</t>
@@ -147,6 +144,12 @@
   </si>
   <si>
     <t>J:1</t>
+  </si>
+  <si>
+    <t>T:1</t>
+  </si>
+  <si>
+    <t>T:2</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1495,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3328,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDF196-0978-4E31-AD1C-547BFF446FB7}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -3392,13 +3395,13 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3415,13 +3418,13 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3432,7 +3435,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
@@ -3443,7 +3446,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3454,7 +3457,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D5" s="8">
         <v>3</v>
@@ -3466,7 +3469,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3476,7 +3479,9 @@
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D6" s="8">
         <v>3</v>
       </c>
@@ -3486,7 +3491,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -3497,7 +3502,9 @@
       <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="8">
         <v>3</v>
       </c>
@@ -3507,7 +3514,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L7" s="2"/>
     </row>
@@ -3518,7 +3525,9 @@
       <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D8" s="8">
         <v>3</v>
       </c>
@@ -3537,7 +3546,9 @@
       <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="8">
         <v>3</v>
       </c>
@@ -3555,7 +3566,9 @@
       <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D10" s="8">
         <v>2</v>
       </c>
@@ -3574,7 +3587,9 @@
       <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="8">
         <v>2</v>
       </c>
@@ -3593,7 +3608,9 @@
       <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
@@ -3612,7 +3629,9 @@
       <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D13" s="2">
         <v>2</v>
       </c>
@@ -3628,7 +3647,7 @@
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5">
         <f>SUBTOTAL(109,Table1[Story Points])</f>
@@ -3647,7 +3666,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3">
         <v>38</v>
@@ -3807,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C753B29C-8070-48CF-BECE-85E4DF604635}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3818,36 +3837,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>38</v>
@@ -3855,7 +3874,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3884,7 +3903,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>38</v>
@@ -3913,7 +3932,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>38</v>
@@ -3937,7 +3956,7 @@
         <v>26</v>
       </c>
       <c r="I5">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>